<commit_message>
Worked out some more changes to the site
</commit_message>
<xml_diff>
--- a/CastleFloorPlan.xlsx
+++ b/CastleFloorPlan.xlsx
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C10:HB171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BM74" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="25" workbookViewId="0">
-      <selection activeCell="BO32" sqref="BO32"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="25" workbookViewId="0">
+      <selection activeCell="GZ72" sqref="A72:GZ72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8590,7 +8590,8 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <webPublishItems count="1">
+  <webPublishItems count="2">
+    <webPublishItem id="25449" divId="CastleFloorPlan_25449" sourceType="sheet" destinationFile="D:\code\TanethPVE\CastleFloorPlan2.htm"/>
     <webPublishItem id="4131" divId="CastleFloorPlan_4131" sourceType="range" sourceRef="B2:HE173" destinationFile="D:\code\TanethPVE\Temp\CastleFloorPlan.htm"/>
   </webPublishItems>
 </worksheet>

</xml_diff>

<commit_message>
More changes before build starts
</commit_message>
<xml_diff>
--- a/CastleFloorPlan.xlsx
+++ b/CastleFloorPlan.xlsx
@@ -19,9 +19,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Wizard Tower</t>
+  </si>
+  <si>
+    <t>Underground Chests - Finished Material</t>
+  </si>
+  <si>
+    <t>Furnace and Raw Cobble/Ore</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>SUBWAY</t>
+  </si>
+  <si>
+    <t>ENTRANCE</t>
   </si>
 </sst>
 </file>
@@ -51,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,8 +121,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -198,11 +243,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -263,6 +345,54 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,7 +666,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -546,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C10:HB171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="40" zoomScaleNormal="40" zoomScaleSheetLayoutView="25" workbookViewId="0">
-      <selection activeCell="GZ72" sqref="A72:GZ72"/>
+    <sheetView tabSelected="1" topLeftCell="T96" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="25" workbookViewId="0">
+      <selection activeCell="ER136" sqref="ER136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,6 +1794,30 @@
       <c r="AK79" s="2"/>
       <c r="AS79" s="2"/>
       <c r="BM79" s="2"/>
+      <c r="CK79" s="25"/>
+      <c r="CL79" s="25"/>
+      <c r="CM79" s="25"/>
+      <c r="CN79" s="25"/>
+      <c r="CO79" s="25"/>
+      <c r="CP79" s="25"/>
+      <c r="CQ79" s="25"/>
+      <c r="CR79" s="25"/>
+      <c r="CS79" s="25"/>
+      <c r="CT79" s="25"/>
+      <c r="CU79" s="25"/>
+      <c r="CV79" s="25"/>
+      <c r="CW79" s="25"/>
+      <c r="CX79" s="25"/>
+      <c r="CY79" s="25"/>
+      <c r="CZ79" s="25"/>
+      <c r="DE79" s="25"/>
+      <c r="DF79" s="25"/>
+      <c r="DG79" s="25"/>
+      <c r="DH79" s="25"/>
+      <c r="DI79" s="25"/>
+      <c r="DJ79" s="25"/>
+      <c r="DK79" s="25"/>
+      <c r="DL79" s="25"/>
       <c r="ER79" s="2"/>
       <c r="FL79" s="2"/>
       <c r="FT79" s="2"/>
@@ -1689,6 +1843,32 @@
       <c r="AL80" s="2"/>
       <c r="AT80" s="2"/>
       <c r="BM80" s="2"/>
+      <c r="CK80" s="25"/>
+      <c r="CL80" s="25"/>
+      <c r="CM80" s="25"/>
+      <c r="CN80" s="25"/>
+      <c r="CO80" s="25"/>
+      <c r="CP80" s="25"/>
+      <c r="CQ80" s="25"/>
+      <c r="CR80" s="25"/>
+      <c r="CS80" s="25"/>
+      <c r="CT80" s="25"/>
+      <c r="CU80" s="25"/>
+      <c r="CV80" s="25"/>
+      <c r="CW80" s="25"/>
+      <c r="CX80" s="25"/>
+      <c r="CY80" s="25"/>
+      <c r="CZ80" s="25"/>
+      <c r="DE80" s="25"/>
+      <c r="DF80" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="DG80" s="31"/>
+      <c r="DH80" s="31"/>
+      <c r="DI80" s="31"/>
+      <c r="DJ80" s="31"/>
+      <c r="DK80" s="32"/>
+      <c r="DL80" s="25"/>
       <c r="ER80" s="2"/>
       <c r="FK80" s="2"/>
       <c r="FS80" s="2"/>
@@ -1714,6 +1894,32 @@
       <c r="AL81" s="2"/>
       <c r="AT81" s="2"/>
       <c r="BM81" s="2"/>
+      <c r="CK81" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="CL81" s="28"/>
+      <c r="CM81" s="28"/>
+      <c r="CN81" s="28"/>
+      <c r="CO81" s="28"/>
+      <c r="CP81" s="28"/>
+      <c r="CQ81" s="28"/>
+      <c r="CR81" s="28"/>
+      <c r="CS81" s="28"/>
+      <c r="CT81" s="28"/>
+      <c r="CU81" s="28"/>
+      <c r="CV81" s="28"/>
+      <c r="CW81" s="28"/>
+      <c r="CX81" s="28"/>
+      <c r="CY81" s="28"/>
+      <c r="CZ81" s="29"/>
+      <c r="DE81" s="25"/>
+      <c r="DF81" s="33"/>
+      <c r="DG81" s="34"/>
+      <c r="DH81" s="34"/>
+      <c r="DI81" s="34"/>
+      <c r="DJ81" s="34"/>
+      <c r="DK81" s="35"/>
+      <c r="DL81" s="25"/>
       <c r="ER81" s="2"/>
       <c r="FK81" s="2"/>
       <c r="FS81" s="2"/>
@@ -1736,6 +1942,30 @@
       <c r="AL82" s="2"/>
       <c r="AT82" s="2"/>
       <c r="BM82" s="2"/>
+      <c r="CK82" s="25"/>
+      <c r="CL82" s="25"/>
+      <c r="CM82" s="25"/>
+      <c r="CN82" s="25"/>
+      <c r="CO82" s="25"/>
+      <c r="CP82" s="25"/>
+      <c r="CQ82" s="25"/>
+      <c r="CR82" s="25"/>
+      <c r="CS82" s="25"/>
+      <c r="CT82" s="25"/>
+      <c r="CU82" s="25"/>
+      <c r="CV82" s="25"/>
+      <c r="CW82" s="25"/>
+      <c r="CX82" s="25"/>
+      <c r="CY82" s="25"/>
+      <c r="CZ82" s="25"/>
+      <c r="DE82" s="25"/>
+      <c r="DF82" s="36"/>
+      <c r="DG82" s="37"/>
+      <c r="DH82" s="37"/>
+      <c r="DI82" s="37"/>
+      <c r="DJ82" s="37"/>
+      <c r="DK82" s="38"/>
+      <c r="DL82" s="25"/>
       <c r="ER82" s="2"/>
       <c r="FK82" s="2"/>
       <c r="FS82" s="2"/>
@@ -1758,6 +1988,30 @@
       <c r="AM83" s="2"/>
       <c r="AU83" s="2"/>
       <c r="BM83" s="2"/>
+      <c r="CK83" s="25"/>
+      <c r="CL83" s="25"/>
+      <c r="CM83" s="25"/>
+      <c r="CN83" s="25"/>
+      <c r="CO83" s="25"/>
+      <c r="CP83" s="25"/>
+      <c r="CQ83" s="25"/>
+      <c r="CR83" s="25"/>
+      <c r="CS83" s="25"/>
+      <c r="CT83" s="25"/>
+      <c r="CU83" s="25"/>
+      <c r="CV83" s="25"/>
+      <c r="CW83" s="25"/>
+      <c r="CX83" s="25"/>
+      <c r="CY83" s="25"/>
+      <c r="CZ83" s="25"/>
+      <c r="DE83" s="25"/>
+      <c r="DF83" s="25"/>
+      <c r="DG83" s="25"/>
+      <c r="DH83" s="25"/>
+      <c r="DI83" s="25"/>
+      <c r="DJ83" s="25"/>
+      <c r="DK83" s="25"/>
+      <c r="DL83" s="25"/>
       <c r="ER83" s="2"/>
       <c r="FJ83" s="2"/>
       <c r="FR83" s="2"/>
@@ -1780,6 +2034,10 @@
       <c r="AM84" s="2"/>
       <c r="AU84" s="2"/>
       <c r="BM84" s="2"/>
+      <c r="DA84" s="26"/>
+      <c r="DB84" s="26"/>
+      <c r="DC84" s="26"/>
+      <c r="DD84" s="26"/>
       <c r="ER84" s="2"/>
       <c r="FJ84" s="2"/>
       <c r="FR84" s="2"/>
@@ -1802,6 +2060,12 @@
       <c r="AM85" s="2"/>
       <c r="AU85" s="2"/>
       <c r="BM85" s="2"/>
+      <c r="DA85" s="26"/>
+      <c r="DB85" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="DC85" s="26"/>
+      <c r="DD85" s="26"/>
       <c r="ER85" s="2"/>
       <c r="FJ85" s="2"/>
       <c r="FR85" s="2"/>
@@ -1833,6 +2097,12 @@
       <c r="CC86" s="2"/>
       <c r="CD86" s="2"/>
       <c r="CE86" s="2"/>
+      <c r="DA86" s="26"/>
+      <c r="DB86" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="DC86" s="26"/>
+      <c r="DD86" s="26"/>
       <c r="DZ86" s="2"/>
       <c r="EA86" s="2"/>
       <c r="EB86" s="2"/>
@@ -1882,6 +2152,12 @@
       <c r="CM87" s="2"/>
       <c r="CN87" s="2"/>
       <c r="CO87" s="2"/>
+      <c r="DA87" s="26"/>
+      <c r="DB87" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="DC87" s="26"/>
+      <c r="DD87" s="26"/>
       <c r="DP87" s="2"/>
       <c r="DQ87" s="2"/>
       <c r="DR87" s="2"/>
@@ -1922,6 +2198,12 @@
       <c r="AN88" s="2"/>
       <c r="AV88" s="2"/>
       <c r="CO88" s="2"/>
+      <c r="DA88" s="26"/>
+      <c r="DB88" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="DC88" s="26"/>
+      <c r="DD88" s="26"/>
       <c r="DP88" s="2"/>
       <c r="FI88" s="2"/>
       <c r="FQ88" s="2"/>
@@ -1944,6 +2226,12 @@
       <c r="AO89" s="2"/>
       <c r="AW89" s="2"/>
       <c r="CO89" s="2"/>
+      <c r="DA89" s="26"/>
+      <c r="DB89" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="DC89" s="26"/>
+      <c r="DD89" s="26"/>
       <c r="DP89" s="2"/>
       <c r="FH89" s="2"/>
       <c r="FP89" s="2"/>
@@ -1966,6 +2254,12 @@
       <c r="AO90" s="2"/>
       <c r="AW90" s="2"/>
       <c r="CO90" s="2"/>
+      <c r="DA90" s="26"/>
+      <c r="DB90" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="DC90" s="26"/>
+      <c r="DD90" s="26"/>
       <c r="DP90" s="2"/>
       <c r="FH90" s="2"/>
       <c r="FP90" s="2"/>
@@ -1988,6 +2282,10 @@
       <c r="AO91" s="2"/>
       <c r="AW91" s="2"/>
       <c r="CO91" s="2"/>
+      <c r="DA91" s="26"/>
+      <c r="DB91" s="26"/>
+      <c r="DC91" s="26"/>
+      <c r="DD91" s="26"/>
       <c r="DP91" s="2"/>
       <c r="FH91" s="2"/>
       <c r="FP91" s="2"/>
@@ -4177,14 +4475,14 @@
       <c r="EI129" s="6"/>
       <c r="EJ129" s="6"/>
       <c r="EK129" s="6"/>
-      <c r="EL129" s="6"/>
-      <c r="EM129" s="6"/>
-      <c r="EN129" s="6"/>
-      <c r="EO129" s="6"/>
-      <c r="EP129" s="6"/>
-      <c r="EQ129" s="6"/>
-      <c r="ER129" s="6"/>
-      <c r="ES129" s="6"/>
+      <c r="EL129" s="39"/>
+      <c r="EM129" s="39"/>
+      <c r="EN129" s="39"/>
+      <c r="EO129" s="39"/>
+      <c r="EP129" s="39"/>
+      <c r="EQ129" s="39"/>
+      <c r="ER129" s="39"/>
+      <c r="ES129" s="39"/>
       <c r="ET129" s="6"/>
       <c r="EU129" s="6"/>
       <c r="EV129" s="6"/>
@@ -4332,14 +4630,14 @@
       <c r="EI130" s="6"/>
       <c r="EJ130" s="6"/>
       <c r="EK130" s="6"/>
-      <c r="EL130" s="6"/>
-      <c r="EM130" s="6"/>
-      <c r="EN130" s="6"/>
-      <c r="EO130" s="6"/>
-      <c r="EP130" s="6"/>
-      <c r="EQ130" s="6"/>
-      <c r="ER130" s="6"/>
-      <c r="ES130" s="6"/>
+      <c r="EL130" s="39"/>
+      <c r="EM130" s="39"/>
+      <c r="EN130" s="39"/>
+      <c r="EO130" s="39"/>
+      <c r="EP130" s="39"/>
+      <c r="EQ130" s="39"/>
+      <c r="ER130" s="39"/>
+      <c r="ES130" s="39"/>
       <c r="ET130" s="6"/>
       <c r="EU130" s="6"/>
       <c r="EV130" s="6"/>
@@ -4484,14 +4782,16 @@
       <c r="EI131" s="6"/>
       <c r="EJ131" s="6"/>
       <c r="EK131" s="6"/>
-      <c r="EL131" s="6"/>
-      <c r="EM131" s="6"/>
-      <c r="EN131" s="6"/>
-      <c r="EO131" s="6"/>
-      <c r="EP131" s="6"/>
-      <c r="EQ131" s="6"/>
-      <c r="ER131" s="6"/>
-      <c r="ES131" s="6"/>
+      <c r="EL131" s="39"/>
+      <c r="EM131" s="39"/>
+      <c r="EN131" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="EO131" s="41"/>
+      <c r="EP131" s="41"/>
+      <c r="EQ131" s="42"/>
+      <c r="ER131" s="39"/>
+      <c r="ES131" s="39"/>
       <c r="ET131" s="6"/>
       <c r="EU131" s="6"/>
       <c r="EV131" s="6"/>
@@ -4643,14 +4943,16 @@
       <c r="EI132" s="6"/>
       <c r="EJ132" s="6"/>
       <c r="EK132" s="6"/>
-      <c r="EL132" s="6"/>
-      <c r="EM132" s="6"/>
-      <c r="EN132" s="6"/>
-      <c r="EO132" s="6"/>
-      <c r="EP132" s="6"/>
-      <c r="EQ132" s="6"/>
-      <c r="ER132" s="6"/>
-      <c r="ES132" s="6"/>
+      <c r="EL132" s="39"/>
+      <c r="EM132" s="39"/>
+      <c r="EN132" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="EO132" s="41"/>
+      <c r="EP132" s="41"/>
+      <c r="EQ132" s="42"/>
+      <c r="ER132" s="39"/>
+      <c r="ES132" s="39"/>
       <c r="ET132" s="6"/>
       <c r="EU132" s="6"/>
       <c r="EV132" s="6"/>
@@ -4802,14 +5104,14 @@
       <c r="EI133" s="6"/>
       <c r="EJ133" s="6"/>
       <c r="EK133" s="6"/>
-      <c r="EL133" s="6"/>
-      <c r="EM133" s="6"/>
-      <c r="EN133" s="6"/>
-      <c r="EO133" s="6"/>
-      <c r="EP133" s="6"/>
-      <c r="EQ133" s="6"/>
-      <c r="ER133" s="6"/>
-      <c r="ES133" s="6"/>
+      <c r="EL133" s="39"/>
+      <c r="EM133" s="39"/>
+      <c r="EN133" s="39"/>
+      <c r="EO133" s="39"/>
+      <c r="EP133" s="39"/>
+      <c r="EQ133" s="39"/>
+      <c r="ER133" s="39"/>
+      <c r="ES133" s="39"/>
       <c r="ET133" s="6"/>
       <c r="EU133" s="6"/>
       <c r="EV133" s="6"/>
@@ -4961,14 +5263,14 @@
       <c r="EI134" s="6"/>
       <c r="EJ134" s="6"/>
       <c r="EK134" s="6"/>
-      <c r="EL134" s="6"/>
-      <c r="EM134" s="6"/>
-      <c r="EN134" s="6"/>
-      <c r="EO134" s="6"/>
-      <c r="EP134" s="6"/>
-      <c r="EQ134" s="6"/>
-      <c r="ER134" s="6"/>
-      <c r="ES134" s="6"/>
+      <c r="EL134" s="39"/>
+      <c r="EM134" s="39"/>
+      <c r="EN134" s="39"/>
+      <c r="EO134" s="39"/>
+      <c r="EP134" s="39"/>
+      <c r="EQ134" s="39"/>
+      <c r="ER134" s="39"/>
+      <c r="ES134" s="39"/>
       <c r="ET134" s="6"/>
       <c r="EU134" s="6"/>
       <c r="EV134" s="6"/>
@@ -5120,14 +5422,14 @@
       <c r="EI135" s="6"/>
       <c r="EJ135" s="6"/>
       <c r="EK135" s="6"/>
-      <c r="EL135" s="6"/>
-      <c r="EM135" s="6"/>
-      <c r="EN135" s="6"/>
-      <c r="EO135" s="6"/>
-      <c r="EP135" s="6"/>
-      <c r="EQ135" s="6"/>
-      <c r="ER135" s="6"/>
-      <c r="ES135" s="6"/>
+      <c r="EL135" s="39"/>
+      <c r="EM135" s="39"/>
+      <c r="EN135" s="39"/>
+      <c r="EO135" s="39"/>
+      <c r="EP135" s="39"/>
+      <c r="EQ135" s="39"/>
+      <c r="ER135" s="39"/>
+      <c r="ES135" s="39"/>
       <c r="ET135" s="6"/>
       <c r="EU135" s="6"/>
       <c r="EV135" s="6"/>
@@ -5279,14 +5581,14 @@
       <c r="EI136" s="6"/>
       <c r="EJ136" s="6"/>
       <c r="EK136" s="6"/>
-      <c r="EL136" s="6"/>
-      <c r="EM136" s="6"/>
-      <c r="EN136" s="6"/>
-      <c r="EO136" s="6"/>
-      <c r="EP136" s="6"/>
-      <c r="EQ136" s="6"/>
-      <c r="ER136" s="6"/>
-      <c r="ES136" s="6"/>
+      <c r="EL136" s="39"/>
+      <c r="EM136" s="39"/>
+      <c r="EN136" s="39"/>
+      <c r="EO136" s="39"/>
+      <c r="EP136" s="39"/>
+      <c r="EQ136" s="39"/>
+      <c r="ER136" s="39"/>
+      <c r="ES136" s="39"/>
       <c r="ET136" s="6"/>
       <c r="EU136" s="6"/>
       <c r="EV136" s="6"/>
@@ -5438,14 +5740,14 @@
       <c r="EI137" s="6"/>
       <c r="EJ137" s="6"/>
       <c r="EK137" s="6"/>
-      <c r="EL137" s="6"/>
-      <c r="EM137" s="6"/>
-      <c r="EN137" s="6"/>
-      <c r="EO137" s="6"/>
-      <c r="EP137" s="6"/>
-      <c r="EQ137" s="6"/>
-      <c r="ER137" s="6"/>
-      <c r="ES137" s="6"/>
+      <c r="EL137" s="39"/>
+      <c r="EM137" s="39"/>
+      <c r="EN137" s="39"/>
+      <c r="EO137" s="39"/>
+      <c r="EP137" s="39"/>
+      <c r="EQ137" s="39"/>
+      <c r="ER137" s="39"/>
+      <c r="ES137" s="39"/>
       <c r="ET137" s="6"/>
       <c r="EU137" s="6"/>
       <c r="EV137" s="6"/>
@@ -8584,9 +8886,13 @@
       <c r="DE171" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="EN132:EQ132"/>
     <mergeCell ref="FC34:FK39"/>
     <mergeCell ref="AS33:BB41"/>
+    <mergeCell ref="CK81:CZ81"/>
+    <mergeCell ref="DF80:DK82"/>
+    <mergeCell ref="EN131:EQ131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adding plot notes and modified floor plan
</commit_message>
<xml_diff>
--- a/CastleFloorPlan.xlsx
+++ b/CastleFloorPlan.xlsx
@@ -78,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,6 +136,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -292,6 +304,18 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -346,8 +370,6 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -384,16 +406,8 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C10:HB171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T96" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="25" workbookViewId="0">
-      <selection activeCell="ER136" sqref="ER136"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="25" workbookViewId="0">
+      <selection activeCell="DI40" sqref="DI40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,6 +840,12 @@
       <c r="AT29" s="2"/>
       <c r="BA29" s="2"/>
       <c r="BB29" s="2"/>
+      <c r="CZ29" s="43"/>
+      <c r="DA29" s="43"/>
+      <c r="DB29" s="43"/>
+      <c r="DC29" s="43"/>
+      <c r="DD29" s="43"/>
+      <c r="DE29" s="43"/>
       <c r="FC29" s="2"/>
       <c r="FD29" s="2"/>
       <c r="FK29" s="2"/>
@@ -838,6 +858,10 @@
       <c r="T30" s="2"/>
       <c r="AR30" s="2"/>
       <c r="BC30" s="2"/>
+      <c r="CX30" s="43"/>
+      <c r="CY30" s="43"/>
+      <c r="DF30" s="43"/>
+      <c r="DG30" s="43"/>
       <c r="FB30" s="2"/>
       <c r="FM30" s="2"/>
       <c r="GK30" s="2"/>
@@ -852,6 +876,8 @@
       <c r="CQ31" s="2"/>
       <c r="CR31" s="2"/>
       <c r="CS31" s="2"/>
+      <c r="CW31" s="43"/>
+      <c r="DH31" s="43"/>
       <c r="DL31" s="2"/>
       <c r="DM31" s="2"/>
       <c r="DN31" s="2"/>
@@ -876,10 +902,10 @@
       <c r="CO32" s="2"/>
       <c r="CT32" s="2"/>
       <c r="CU32" s="2"/>
-      <c r="CV32" s="2"/>
-      <c r="CW32" s="2"/>
-      <c r="DH32" s="2"/>
-      <c r="DI32" s="2"/>
+      <c r="CV32" s="43"/>
+      <c r="CW32" s="44"/>
+      <c r="DH32" s="44"/>
+      <c r="DI32" s="43"/>
       <c r="DJ32" s="2"/>
       <c r="DK32" s="2"/>
       <c r="DP32" s="2"/>
@@ -899,18 +925,18 @@
       <c r="O33" s="2"/>
       <c r="S33" s="2"/>
       <c r="AP33" s="2"/>
-      <c r="AS33" s="16" t="s">
+      <c r="AS33" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="AT33" s="17"/>
-      <c r="AU33" s="17"/>
-      <c r="AV33" s="17"/>
-      <c r="AW33" s="17"/>
-      <c r="AX33" s="17"/>
-      <c r="AY33" s="17"/>
-      <c r="AZ33" s="17"/>
-      <c r="BA33" s="17"/>
-      <c r="BB33" s="18"/>
+      <c r="AT33" s="23"/>
+      <c r="AU33" s="23"/>
+      <c r="AV33" s="23"/>
+      <c r="AW33" s="23"/>
+      <c r="AX33" s="23"/>
+      <c r="AY33" s="23"/>
+      <c r="AZ33" s="23"/>
+      <c r="BA33" s="23"/>
+      <c r="BB33" s="24"/>
       <c r="BE33" s="2"/>
       <c r="BJ33" s="2"/>
       <c r="BK33" s="2"/>
@@ -920,16 +946,18 @@
       <c r="CI33" s="2"/>
       <c r="CJ33" s="2"/>
       <c r="CK33" s="2"/>
-      <c r="CX33" s="2"/>
-      <c r="CY33" s="2"/>
-      <c r="CZ33" s="2"/>
-      <c r="DA33" s="2"/>
-      <c r="DB33" s="2"/>
-      <c r="DC33" s="2"/>
-      <c r="DD33" s="2"/>
-      <c r="DE33" s="2"/>
-      <c r="DF33" s="2"/>
-      <c r="DG33" s="2"/>
+      <c r="CU33" s="43"/>
+      <c r="CX33" s="44"/>
+      <c r="CY33" s="44"/>
+      <c r="CZ33" s="43"/>
+      <c r="DA33" s="43"/>
+      <c r="DB33" s="43"/>
+      <c r="DC33" s="43"/>
+      <c r="DD33" s="43"/>
+      <c r="DE33" s="43"/>
+      <c r="DF33" s="44"/>
+      <c r="DG33" s="44"/>
+      <c r="DJ33" s="43"/>
       <c r="DT33" s="2"/>
       <c r="DU33" s="2"/>
       <c r="DV33" s="2"/>
@@ -947,16 +975,16 @@
       <c r="N34" s="2"/>
       <c r="R34" s="2"/>
       <c r="AO34" s="2"/>
-      <c r="AS34" s="19"/>
-      <c r="AT34" s="20"/>
-      <c r="AU34" s="20"/>
-      <c r="AV34" s="20"/>
-      <c r="AW34" s="20"/>
-      <c r="AX34" s="20"/>
-      <c r="AY34" s="20"/>
-      <c r="AZ34" s="20"/>
-      <c r="BA34" s="20"/>
-      <c r="BB34" s="21"/>
+      <c r="AS34" s="25"/>
+      <c r="AT34" s="26"/>
+      <c r="AU34" s="26"/>
+      <c r="AV34" s="26"/>
+      <c r="AW34" s="26"/>
+      <c r="AX34" s="26"/>
+      <c r="AY34" s="26"/>
+      <c r="AZ34" s="26"/>
+      <c r="BA34" s="26"/>
+      <c r="BB34" s="27"/>
       <c r="BF34" s="2"/>
       <c r="BN34" s="2"/>
       <c r="BO34" s="2"/>
@@ -966,6 +994,12 @@
       <c r="CE34" s="2"/>
       <c r="CF34" s="2"/>
       <c r="CG34" s="2"/>
+      <c r="CT34" s="43"/>
+      <c r="CX34" s="43"/>
+      <c r="CY34" s="43"/>
+      <c r="DF34" s="43"/>
+      <c r="DG34" s="43"/>
+      <c r="DK34" s="43"/>
       <c r="DX34" s="2"/>
       <c r="DY34" s="2"/>
       <c r="DZ34" s="2"/>
@@ -975,17 +1009,17 @@
       <c r="EP34" s="2"/>
       <c r="EQ34" s="2"/>
       <c r="EY34" s="2"/>
-      <c r="FC34" s="7" t="s">
+      <c r="FC34" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="FD34" s="8"/>
-      <c r="FE34" s="8"/>
-      <c r="FF34" s="8"/>
-      <c r="FG34" s="8"/>
-      <c r="FH34" s="8"/>
-      <c r="FI34" s="8"/>
-      <c r="FJ34" s="8"/>
-      <c r="FK34" s="9"/>
+      <c r="FD34" s="14"/>
+      <c r="FE34" s="14"/>
+      <c r="FF34" s="14"/>
+      <c r="FG34" s="14"/>
+      <c r="FH34" s="14"/>
+      <c r="FI34" s="14"/>
+      <c r="FJ34" s="14"/>
+      <c r="FK34" s="15"/>
       <c r="FP34" s="2"/>
       <c r="GM34" s="2"/>
       <c r="GQ34" s="2"/>
@@ -994,16 +1028,16 @@
       <c r="N35" s="2"/>
       <c r="R35" s="2"/>
       <c r="AO35" s="2"/>
-      <c r="AS35" s="19"/>
-      <c r="AT35" s="20"/>
-      <c r="AU35" s="20"/>
-      <c r="AV35" s="20"/>
-      <c r="AW35" s="20"/>
-      <c r="AX35" s="20"/>
-      <c r="AY35" s="20"/>
-      <c r="AZ35" s="20"/>
-      <c r="BA35" s="20"/>
-      <c r="BB35" s="21"/>
+      <c r="AS35" s="25"/>
+      <c r="AT35" s="26"/>
+      <c r="AU35" s="26"/>
+      <c r="AV35" s="26"/>
+      <c r="AW35" s="26"/>
+      <c r="AX35" s="26"/>
+      <c r="AY35" s="26"/>
+      <c r="AZ35" s="26"/>
+      <c r="BA35" s="26"/>
+      <c r="BB35" s="27"/>
       <c r="BF35" s="2"/>
       <c r="BR35" s="2"/>
       <c r="BS35" s="2"/>
@@ -1013,6 +1047,10 @@
       <c r="CA35" s="2"/>
       <c r="CB35" s="2"/>
       <c r="CC35" s="2"/>
+      <c r="CT35" s="43"/>
+      <c r="CW35" s="43"/>
+      <c r="DH35" s="43"/>
+      <c r="DK35" s="43"/>
       <c r="EB35" s="2"/>
       <c r="EC35" s="2"/>
       <c r="ED35" s="2"/>
@@ -1022,15 +1060,15 @@
       <c r="EL35" s="2"/>
       <c r="EM35" s="2"/>
       <c r="EY35" s="2"/>
-      <c r="FC35" s="10"/>
-      <c r="FD35" s="11"/>
-      <c r="FE35" s="11"/>
-      <c r="FF35" s="11"/>
-      <c r="FG35" s="11"/>
-      <c r="FH35" s="11"/>
-      <c r="FI35" s="11"/>
-      <c r="FJ35" s="11"/>
-      <c r="FK35" s="12"/>
+      <c r="FC35" s="16"/>
+      <c r="FD35" s="17"/>
+      <c r="FE35" s="17"/>
+      <c r="FF35" s="17"/>
+      <c r="FG35" s="17"/>
+      <c r="FH35" s="17"/>
+      <c r="FI35" s="17"/>
+      <c r="FJ35" s="17"/>
+      <c r="FK35" s="18"/>
       <c r="FP35" s="2"/>
       <c r="GM35" s="2"/>
       <c r="GQ35" s="2"/>
@@ -1039,35 +1077,39 @@
       <c r="M36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="AO36" s="2"/>
-      <c r="AS36" s="19"/>
-      <c r="AT36" s="20"/>
-      <c r="AU36" s="20"/>
-      <c r="AV36" s="20"/>
-      <c r="AW36" s="20"/>
-      <c r="AX36" s="20"/>
-      <c r="AY36" s="20"/>
-      <c r="AZ36" s="20"/>
-      <c r="BA36" s="20"/>
-      <c r="BB36" s="21"/>
+      <c r="AS36" s="25"/>
+      <c r="AT36" s="26"/>
+      <c r="AU36" s="26"/>
+      <c r="AV36" s="26"/>
+      <c r="AW36" s="26"/>
+      <c r="AX36" s="26"/>
+      <c r="AY36" s="26"/>
+      <c r="AZ36" s="26"/>
+      <c r="BA36" s="26"/>
+      <c r="BB36" s="27"/>
       <c r="BF36" s="2"/>
       <c r="BV36" s="2"/>
       <c r="BW36" s="2"/>
       <c r="BX36" s="2"/>
       <c r="BY36" s="2"/>
+      <c r="CS36" s="43"/>
+      <c r="CV36" s="43"/>
+      <c r="DI36" s="43"/>
+      <c r="DL36" s="43"/>
       <c r="EF36" s="2"/>
       <c r="EG36" s="2"/>
       <c r="EH36" s="2"/>
       <c r="EI36" s="2"/>
       <c r="EY36" s="2"/>
-      <c r="FC36" s="10"/>
-      <c r="FD36" s="11"/>
-      <c r="FE36" s="11"/>
-      <c r="FF36" s="11"/>
-      <c r="FG36" s="11"/>
-      <c r="FH36" s="11"/>
-      <c r="FI36" s="11"/>
-      <c r="FJ36" s="11"/>
-      <c r="FK36" s="12"/>
+      <c r="FC36" s="16"/>
+      <c r="FD36" s="17"/>
+      <c r="FE36" s="17"/>
+      <c r="FF36" s="17"/>
+      <c r="FG36" s="17"/>
+      <c r="FH36" s="17"/>
+      <c r="FI36" s="17"/>
+      <c r="FJ36" s="17"/>
+      <c r="FK36" s="18"/>
       <c r="FP36" s="2"/>
       <c r="GN36" s="2"/>
       <c r="GR36" s="2"/>
@@ -1076,27 +1118,31 @@
       <c r="M37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="AO37" s="2"/>
-      <c r="AS37" s="19"/>
-      <c r="AT37" s="20"/>
-      <c r="AU37" s="20"/>
-      <c r="AV37" s="20"/>
-      <c r="AW37" s="20"/>
-      <c r="AX37" s="20"/>
-      <c r="AY37" s="20"/>
-      <c r="AZ37" s="20"/>
-      <c r="BA37" s="20"/>
-      <c r="BB37" s="21"/>
+      <c r="AS37" s="25"/>
+      <c r="AT37" s="26"/>
+      <c r="AU37" s="26"/>
+      <c r="AV37" s="26"/>
+      <c r="AW37" s="26"/>
+      <c r="AX37" s="26"/>
+      <c r="AY37" s="26"/>
+      <c r="AZ37" s="26"/>
+      <c r="BA37" s="26"/>
+      <c r="BB37" s="27"/>
       <c r="BF37" s="2"/>
+      <c r="CS37" s="43"/>
+      <c r="CV37" s="43"/>
+      <c r="DI37" s="43"/>
+      <c r="DL37" s="43"/>
       <c r="EY37" s="2"/>
-      <c r="FC37" s="10"/>
-      <c r="FD37" s="11"/>
-      <c r="FE37" s="11"/>
-      <c r="FF37" s="11"/>
-      <c r="FG37" s="11"/>
-      <c r="FH37" s="11"/>
-      <c r="FI37" s="11"/>
-      <c r="FJ37" s="11"/>
-      <c r="FK37" s="12"/>
+      <c r="FC37" s="16"/>
+      <c r="FD37" s="17"/>
+      <c r="FE37" s="17"/>
+      <c r="FF37" s="17"/>
+      <c r="FG37" s="17"/>
+      <c r="FH37" s="17"/>
+      <c r="FI37" s="17"/>
+      <c r="FJ37" s="17"/>
+      <c r="FK37" s="18"/>
       <c r="FP37" s="2"/>
       <c r="GN37" s="2"/>
       <c r="GR37" s="2"/>
@@ -1105,27 +1151,31 @@
       <c r="L38" s="2"/>
       <c r="P38" s="2"/>
       <c r="AO38" s="2"/>
-      <c r="AS38" s="19"/>
-      <c r="AT38" s="20"/>
-      <c r="AU38" s="20"/>
-      <c r="AV38" s="20"/>
-      <c r="AW38" s="20"/>
-      <c r="AX38" s="20"/>
-      <c r="AY38" s="20"/>
-      <c r="AZ38" s="20"/>
-      <c r="BA38" s="20"/>
-      <c r="BB38" s="21"/>
+      <c r="AS38" s="25"/>
+      <c r="AT38" s="26"/>
+      <c r="AU38" s="26"/>
+      <c r="AV38" s="26"/>
+      <c r="AW38" s="26"/>
+      <c r="AX38" s="26"/>
+      <c r="AY38" s="26"/>
+      <c r="AZ38" s="26"/>
+      <c r="BA38" s="26"/>
+      <c r="BB38" s="27"/>
       <c r="BF38" s="2"/>
+      <c r="CS38" s="43"/>
+      <c r="CV38" s="43"/>
+      <c r="DI38" s="43"/>
+      <c r="DL38" s="43"/>
       <c r="EY38" s="2"/>
-      <c r="FC38" s="10"/>
-      <c r="FD38" s="11"/>
-      <c r="FE38" s="11"/>
-      <c r="FF38" s="11"/>
-      <c r="FG38" s="11"/>
-      <c r="FH38" s="11"/>
-      <c r="FI38" s="11"/>
-      <c r="FJ38" s="11"/>
-      <c r="FK38" s="12"/>
+      <c r="FC38" s="16"/>
+      <c r="FD38" s="17"/>
+      <c r="FE38" s="17"/>
+      <c r="FF38" s="17"/>
+      <c r="FG38" s="17"/>
+      <c r="FH38" s="17"/>
+      <c r="FI38" s="17"/>
+      <c r="FJ38" s="17"/>
+      <c r="FK38" s="18"/>
       <c r="FP38" s="2"/>
       <c r="GO38" s="2"/>
       <c r="GS38" s="2"/>
@@ -1134,35 +1184,37 @@
       <c r="L39" s="2"/>
       <c r="P39" s="2"/>
       <c r="AO39" s="2"/>
-      <c r="AS39" s="19"/>
-      <c r="AT39" s="20"/>
-      <c r="AU39" s="20"/>
-      <c r="AV39" s="20"/>
-      <c r="AW39" s="20"/>
-      <c r="AX39" s="20"/>
-      <c r="AY39" s="20"/>
-      <c r="AZ39" s="20"/>
-      <c r="BA39" s="20"/>
-      <c r="BB39" s="21"/>
+      <c r="AS39" s="25"/>
+      <c r="AT39" s="26"/>
+      <c r="AU39" s="26"/>
+      <c r="AV39" s="26"/>
+      <c r="AW39" s="26"/>
+      <c r="AX39" s="26"/>
+      <c r="AY39" s="26"/>
+      <c r="AZ39" s="26"/>
+      <c r="BA39" s="26"/>
+      <c r="BB39" s="27"/>
       <c r="BF39" s="2"/>
       <c r="CP39" s="2"/>
       <c r="CQ39" s="2"/>
       <c r="CR39" s="2"/>
-      <c r="CS39" s="2"/>
-      <c r="DL39" s="2"/>
+      <c r="CS39" s="43"/>
+      <c r="CV39" s="43"/>
+      <c r="DI39" s="43"/>
+      <c r="DL39" s="43"/>
       <c r="DM39" s="2"/>
       <c r="DN39" s="2"/>
       <c r="DO39" s="2"/>
       <c r="EY39" s="2"/>
-      <c r="FC39" s="13"/>
-      <c r="FD39" s="14"/>
-      <c r="FE39" s="14"/>
-      <c r="FF39" s="14"/>
-      <c r="FG39" s="14"/>
-      <c r="FH39" s="14"/>
-      <c r="FI39" s="14"/>
-      <c r="FJ39" s="14"/>
-      <c r="FK39" s="15"/>
+      <c r="FC39" s="19"/>
+      <c r="FD39" s="20"/>
+      <c r="FE39" s="20"/>
+      <c r="FF39" s="20"/>
+      <c r="FG39" s="20"/>
+      <c r="FH39" s="20"/>
+      <c r="FI39" s="20"/>
+      <c r="FJ39" s="20"/>
+      <c r="FK39" s="21"/>
       <c r="FP39" s="2"/>
       <c r="GO39" s="2"/>
       <c r="GS39" s="2"/>
@@ -1171,16 +1223,16 @@
       <c r="K40" s="2"/>
       <c r="O40" s="2"/>
       <c r="AP40" s="2"/>
-      <c r="AS40" s="19"/>
-      <c r="AT40" s="20"/>
-      <c r="AU40" s="20"/>
-      <c r="AV40" s="20"/>
-      <c r="AW40" s="20"/>
-      <c r="AX40" s="20"/>
-      <c r="AY40" s="20"/>
-      <c r="AZ40" s="20"/>
-      <c r="BA40" s="20"/>
-      <c r="BB40" s="21"/>
+      <c r="AS40" s="25"/>
+      <c r="AT40" s="26"/>
+      <c r="AU40" s="26"/>
+      <c r="AV40" s="26"/>
+      <c r="AW40" s="26"/>
+      <c r="AX40" s="26"/>
+      <c r="AY40" s="26"/>
+      <c r="AZ40" s="26"/>
+      <c r="BA40" s="26"/>
+      <c r="BB40" s="27"/>
       <c r="BE40" s="2"/>
       <c r="BG40" s="2"/>
       <c r="BH40" s="2"/>
@@ -1192,9 +1244,19 @@
       <c r="CT40" s="2"/>
       <c r="CU40" s="2"/>
       <c r="CV40" s="2"/>
-      <c r="CW40" s="2"/>
-      <c r="DH40" s="2"/>
-      <c r="DI40" s="2"/>
+      <c r="CW40" s="44"/>
+      <c r="CX40" s="44"/>
+      <c r="CY40" s="44"/>
+      <c r="CZ40" s="44"/>
+      <c r="DA40" s="44"/>
+      <c r="DB40" s="44"/>
+      <c r="DC40" s="44"/>
+      <c r="DD40" s="44"/>
+      <c r="DE40" s="44"/>
+      <c r="DF40" s="44"/>
+      <c r="DG40" s="44"/>
+      <c r="DH40" s="44"/>
+      <c r="DI40" s="43"/>
       <c r="DJ40" s="2"/>
       <c r="DK40" s="2"/>
       <c r="DP40" s="2"/>
@@ -1214,16 +1276,16 @@
       <c r="K41" s="2"/>
       <c r="O41" s="2"/>
       <c r="AP41" s="2"/>
-      <c r="AS41" s="22"/>
-      <c r="AT41" s="23"/>
-      <c r="AU41" s="23"/>
-      <c r="AV41" s="23"/>
-      <c r="AW41" s="23"/>
-      <c r="AX41" s="23"/>
-      <c r="AY41" s="23"/>
-      <c r="AZ41" s="23"/>
-      <c r="BA41" s="23"/>
-      <c r="BB41" s="24"/>
+      <c r="AS41" s="28"/>
+      <c r="AT41" s="29"/>
+      <c r="AU41" s="29"/>
+      <c r="AV41" s="29"/>
+      <c r="AW41" s="29"/>
+      <c r="AX41" s="29"/>
+      <c r="AY41" s="29"/>
+      <c r="AZ41" s="29"/>
+      <c r="BA41" s="29"/>
+      <c r="BB41" s="30"/>
       <c r="BE41" s="2"/>
       <c r="BJ41" s="2"/>
       <c r="BK41" s="2"/>
@@ -1233,16 +1295,18 @@
       <c r="CI41" s="2"/>
       <c r="CJ41" s="2"/>
       <c r="CK41" s="2"/>
-      <c r="CX41" s="2"/>
-      <c r="CY41" s="2"/>
-      <c r="CZ41" s="2"/>
-      <c r="DA41" s="2"/>
-      <c r="DB41" s="2"/>
-      <c r="DC41" s="2"/>
-      <c r="DD41" s="2"/>
-      <c r="DE41" s="2"/>
-      <c r="DF41" s="2"/>
-      <c r="DG41" s="2"/>
+      <c r="CW41" s="44"/>
+      <c r="CX41" s="44"/>
+      <c r="CY41" s="44"/>
+      <c r="CZ41" s="44"/>
+      <c r="DA41" s="44"/>
+      <c r="DB41" s="44"/>
+      <c r="DC41" s="44"/>
+      <c r="DD41" s="44"/>
+      <c r="DE41" s="44"/>
+      <c r="DF41" s="44"/>
+      <c r="DG41" s="44"/>
+      <c r="DH41" s="44"/>
       <c r="DT41" s="2"/>
       <c r="DU41" s="2"/>
       <c r="DV41" s="2"/>
@@ -1270,6 +1334,18 @@
       <c r="CE42" s="2"/>
       <c r="CF42" s="2"/>
       <c r="CG42" s="2"/>
+      <c r="CW42" s="44"/>
+      <c r="CX42" s="44"/>
+      <c r="CY42" s="44"/>
+      <c r="CZ42" s="44"/>
+      <c r="DA42" s="44"/>
+      <c r="DB42" s="44"/>
+      <c r="DC42" s="44"/>
+      <c r="DD42" s="44"/>
+      <c r="DE42" s="44"/>
+      <c r="DF42" s="44"/>
+      <c r="DG42" s="44"/>
+      <c r="DH42" s="44"/>
       <c r="DX42" s="2"/>
       <c r="DY42" s="2"/>
       <c r="DZ42" s="2"/>
@@ -1794,30 +1870,30 @@
       <c r="AK79" s="2"/>
       <c r="AS79" s="2"/>
       <c r="BM79" s="2"/>
-      <c r="CK79" s="25"/>
-      <c r="CL79" s="25"/>
-      <c r="CM79" s="25"/>
-      <c r="CN79" s="25"/>
-      <c r="CO79" s="25"/>
-      <c r="CP79" s="25"/>
-      <c r="CQ79" s="25"/>
-      <c r="CR79" s="25"/>
-      <c r="CS79" s="25"/>
-      <c r="CT79" s="25"/>
-      <c r="CU79" s="25"/>
-      <c r="CV79" s="25"/>
-      <c r="CW79" s="25"/>
-      <c r="CX79" s="25"/>
-      <c r="CY79" s="25"/>
-      <c r="CZ79" s="25"/>
-      <c r="DE79" s="25"/>
-      <c r="DF79" s="25"/>
-      <c r="DG79" s="25"/>
-      <c r="DH79" s="25"/>
-      <c r="DI79" s="25"/>
-      <c r="DJ79" s="25"/>
-      <c r="DK79" s="25"/>
-      <c r="DL79" s="25"/>
+      <c r="CK79" s="7"/>
+      <c r="CL79" s="7"/>
+      <c r="CM79" s="7"/>
+      <c r="CN79" s="7"/>
+      <c r="CO79" s="7"/>
+      <c r="CP79" s="7"/>
+      <c r="CQ79" s="7"/>
+      <c r="CR79" s="7"/>
+      <c r="CS79" s="7"/>
+      <c r="CT79" s="7"/>
+      <c r="CU79" s="7"/>
+      <c r="CV79" s="7"/>
+      <c r="CW79" s="7"/>
+      <c r="CX79" s="7"/>
+      <c r="CY79" s="7"/>
+      <c r="CZ79" s="7"/>
+      <c r="DE79" s="7"/>
+      <c r="DF79" s="7"/>
+      <c r="DG79" s="7"/>
+      <c r="DH79" s="7"/>
+      <c r="DI79" s="7"/>
+      <c r="DJ79" s="7"/>
+      <c r="DK79" s="7"/>
+      <c r="DL79" s="7"/>
       <c r="ER79" s="2"/>
       <c r="FL79" s="2"/>
       <c r="FT79" s="2"/>
@@ -1843,32 +1919,32 @@
       <c r="AL80" s="2"/>
       <c r="AT80" s="2"/>
       <c r="BM80" s="2"/>
-      <c r="CK80" s="25"/>
-      <c r="CL80" s="25"/>
-      <c r="CM80" s="25"/>
-      <c r="CN80" s="25"/>
-      <c r="CO80" s="25"/>
-      <c r="CP80" s="25"/>
-      <c r="CQ80" s="25"/>
-      <c r="CR80" s="25"/>
-      <c r="CS80" s="25"/>
-      <c r="CT80" s="25"/>
-      <c r="CU80" s="25"/>
-      <c r="CV80" s="25"/>
-      <c r="CW80" s="25"/>
-      <c r="CX80" s="25"/>
-      <c r="CY80" s="25"/>
-      <c r="CZ80" s="25"/>
-      <c r="DE80" s="25"/>
-      <c r="DF80" s="30" t="s">
+      <c r="CK80" s="7"/>
+      <c r="CL80" s="7"/>
+      <c r="CM80" s="7"/>
+      <c r="CN80" s="7"/>
+      <c r="CO80" s="7"/>
+      <c r="CP80" s="7"/>
+      <c r="CQ80" s="7"/>
+      <c r="CR80" s="7"/>
+      <c r="CS80" s="7"/>
+      <c r="CT80" s="7"/>
+      <c r="CU80" s="7"/>
+      <c r="CV80" s="7"/>
+      <c r="CW80" s="7"/>
+      <c r="CX80" s="7"/>
+      <c r="CY80" s="7"/>
+      <c r="CZ80" s="7"/>
+      <c r="DE80" s="7"/>
+      <c r="DF80" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="DG80" s="31"/>
-      <c r="DH80" s="31"/>
-      <c r="DI80" s="31"/>
-      <c r="DJ80" s="31"/>
-      <c r="DK80" s="32"/>
-      <c r="DL80" s="25"/>
+      <c r="DG80" s="35"/>
+      <c r="DH80" s="35"/>
+      <c r="DI80" s="35"/>
+      <c r="DJ80" s="35"/>
+      <c r="DK80" s="36"/>
+      <c r="DL80" s="7"/>
       <c r="ER80" s="2"/>
       <c r="FK80" s="2"/>
       <c r="FS80" s="2"/>
@@ -1894,32 +1970,32 @@
       <c r="AL81" s="2"/>
       <c r="AT81" s="2"/>
       <c r="BM81" s="2"/>
-      <c r="CK81" s="27" t="s">
+      <c r="CK81" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="CL81" s="28"/>
-      <c r="CM81" s="28"/>
-      <c r="CN81" s="28"/>
-      <c r="CO81" s="28"/>
-      <c r="CP81" s="28"/>
-      <c r="CQ81" s="28"/>
-      <c r="CR81" s="28"/>
-      <c r="CS81" s="28"/>
-      <c r="CT81" s="28"/>
-      <c r="CU81" s="28"/>
-      <c r="CV81" s="28"/>
-      <c r="CW81" s="28"/>
-      <c r="CX81" s="28"/>
-      <c r="CY81" s="28"/>
-      <c r="CZ81" s="29"/>
-      <c r="DE81" s="25"/>
-      <c r="DF81" s="33"/>
-      <c r="DG81" s="34"/>
-      <c r="DH81" s="34"/>
-      <c r="DI81" s="34"/>
-      <c r="DJ81" s="34"/>
-      <c r="DK81" s="35"/>
-      <c r="DL81" s="25"/>
+      <c r="CL81" s="32"/>
+      <c r="CM81" s="32"/>
+      <c r="CN81" s="32"/>
+      <c r="CO81" s="32"/>
+      <c r="CP81" s="32"/>
+      <c r="CQ81" s="32"/>
+      <c r="CR81" s="32"/>
+      <c r="CS81" s="32"/>
+      <c r="CT81" s="32"/>
+      <c r="CU81" s="32"/>
+      <c r="CV81" s="32"/>
+      <c r="CW81" s="32"/>
+      <c r="CX81" s="32"/>
+      <c r="CY81" s="32"/>
+      <c r="CZ81" s="33"/>
+      <c r="DE81" s="7"/>
+      <c r="DF81" s="37"/>
+      <c r="DG81" s="38"/>
+      <c r="DH81" s="38"/>
+      <c r="DI81" s="38"/>
+      <c r="DJ81" s="38"/>
+      <c r="DK81" s="39"/>
+      <c r="DL81" s="7"/>
       <c r="ER81" s="2"/>
       <c r="FK81" s="2"/>
       <c r="FS81" s="2"/>
@@ -1942,30 +2018,30 @@
       <c r="AL82" s="2"/>
       <c r="AT82" s="2"/>
       <c r="BM82" s="2"/>
-      <c r="CK82" s="25"/>
-      <c r="CL82" s="25"/>
-      <c r="CM82" s="25"/>
-      <c r="CN82" s="25"/>
-      <c r="CO82" s="25"/>
-      <c r="CP82" s="25"/>
-      <c r="CQ82" s="25"/>
-      <c r="CR82" s="25"/>
-      <c r="CS82" s="25"/>
-      <c r="CT82" s="25"/>
-      <c r="CU82" s="25"/>
-      <c r="CV82" s="25"/>
-      <c r="CW82" s="25"/>
-      <c r="CX82" s="25"/>
-      <c r="CY82" s="25"/>
-      <c r="CZ82" s="25"/>
-      <c r="DE82" s="25"/>
-      <c r="DF82" s="36"/>
-      <c r="DG82" s="37"/>
-      <c r="DH82" s="37"/>
-      <c r="DI82" s="37"/>
-      <c r="DJ82" s="37"/>
-      <c r="DK82" s="38"/>
-      <c r="DL82" s="25"/>
+      <c r="CK82" s="7"/>
+      <c r="CL82" s="7"/>
+      <c r="CM82" s="7"/>
+      <c r="CN82" s="7"/>
+      <c r="CO82" s="7"/>
+      <c r="CP82" s="7"/>
+      <c r="CQ82" s="7"/>
+      <c r="CR82" s="7"/>
+      <c r="CS82" s="7"/>
+      <c r="CT82" s="7"/>
+      <c r="CU82" s="7"/>
+      <c r="CV82" s="7"/>
+      <c r="CW82" s="7"/>
+      <c r="CX82" s="7"/>
+      <c r="CY82" s="7"/>
+      <c r="CZ82" s="7"/>
+      <c r="DE82" s="7"/>
+      <c r="DF82" s="40"/>
+      <c r="DG82" s="41"/>
+      <c r="DH82" s="41"/>
+      <c r="DI82" s="41"/>
+      <c r="DJ82" s="41"/>
+      <c r="DK82" s="42"/>
+      <c r="DL82" s="7"/>
       <c r="ER82" s="2"/>
       <c r="FK82" s="2"/>
       <c r="FS82" s="2"/>
@@ -1988,30 +2064,30 @@
       <c r="AM83" s="2"/>
       <c r="AU83" s="2"/>
       <c r="BM83" s="2"/>
-      <c r="CK83" s="25"/>
-      <c r="CL83" s="25"/>
-      <c r="CM83" s="25"/>
-      <c r="CN83" s="25"/>
-      <c r="CO83" s="25"/>
-      <c r="CP83" s="25"/>
-      <c r="CQ83" s="25"/>
-      <c r="CR83" s="25"/>
-      <c r="CS83" s="25"/>
-      <c r="CT83" s="25"/>
-      <c r="CU83" s="25"/>
-      <c r="CV83" s="25"/>
-      <c r="CW83" s="25"/>
-      <c r="CX83" s="25"/>
-      <c r="CY83" s="25"/>
-      <c r="CZ83" s="25"/>
-      <c r="DE83" s="25"/>
-      <c r="DF83" s="25"/>
-      <c r="DG83" s="25"/>
-      <c r="DH83" s="25"/>
-      <c r="DI83" s="25"/>
-      <c r="DJ83" s="25"/>
-      <c r="DK83" s="25"/>
-      <c r="DL83" s="25"/>
+      <c r="CK83" s="7"/>
+      <c r="CL83" s="7"/>
+      <c r="CM83" s="7"/>
+      <c r="CN83" s="7"/>
+      <c r="CO83" s="7"/>
+      <c r="CP83" s="7"/>
+      <c r="CQ83" s="7"/>
+      <c r="CR83" s="7"/>
+      <c r="CS83" s="7"/>
+      <c r="CT83" s="7"/>
+      <c r="CU83" s="7"/>
+      <c r="CV83" s="7"/>
+      <c r="CW83" s="7"/>
+      <c r="CX83" s="7"/>
+      <c r="CY83" s="7"/>
+      <c r="CZ83" s="7"/>
+      <c r="DE83" s="7"/>
+      <c r="DF83" s="7"/>
+      <c r="DG83" s="7"/>
+      <c r="DH83" s="7"/>
+      <c r="DI83" s="7"/>
+      <c r="DJ83" s="7"/>
+      <c r="DK83" s="7"/>
+      <c r="DL83" s="7"/>
       <c r="ER83" s="2"/>
       <c r="FJ83" s="2"/>
       <c r="FR83" s="2"/>
@@ -2034,10 +2110,10 @@
       <c r="AM84" s="2"/>
       <c r="AU84" s="2"/>
       <c r="BM84" s="2"/>
-      <c r="DA84" s="26"/>
-      <c r="DB84" s="26"/>
-      <c r="DC84" s="26"/>
-      <c r="DD84" s="26"/>
+      <c r="DA84" s="8"/>
+      <c r="DB84" s="8"/>
+      <c r="DC84" s="8"/>
+      <c r="DD84" s="8"/>
       <c r="ER84" s="2"/>
       <c r="FJ84" s="2"/>
       <c r="FR84" s="2"/>
@@ -2060,12 +2136,12 @@
       <c r="AM85" s="2"/>
       <c r="AU85" s="2"/>
       <c r="BM85" s="2"/>
-      <c r="DA85" s="26"/>
-      <c r="DB85" s="26" t="s">
+      <c r="DA85" s="8"/>
+      <c r="DB85" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="DC85" s="26"/>
-      <c r="DD85" s="26"/>
+      <c r="DC85" s="8"/>
+      <c r="DD85" s="8"/>
       <c r="ER85" s="2"/>
       <c r="FJ85" s="2"/>
       <c r="FR85" s="2"/>
@@ -2097,12 +2173,12 @@
       <c r="CC86" s="2"/>
       <c r="CD86" s="2"/>
       <c r="CE86" s="2"/>
-      <c r="DA86" s="26"/>
-      <c r="DB86" s="26" t="s">
+      <c r="DA86" s="8"/>
+      <c r="DB86" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="DC86" s="26"/>
-      <c r="DD86" s="26"/>
+      <c r="DC86" s="8"/>
+      <c r="DD86" s="8"/>
       <c r="DZ86" s="2"/>
       <c r="EA86" s="2"/>
       <c r="EB86" s="2"/>
@@ -2152,12 +2228,12 @@
       <c r="CM87" s="2"/>
       <c r="CN87" s="2"/>
       <c r="CO87" s="2"/>
-      <c r="DA87" s="26"/>
-      <c r="DB87" s="26" t="s">
+      <c r="DA87" s="8"/>
+      <c r="DB87" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="DC87" s="26"/>
-      <c r="DD87" s="26"/>
+      <c r="DC87" s="8"/>
+      <c r="DD87" s="8"/>
       <c r="DP87" s="2"/>
       <c r="DQ87" s="2"/>
       <c r="DR87" s="2"/>
@@ -2198,12 +2274,12 @@
       <c r="AN88" s="2"/>
       <c r="AV88" s="2"/>
       <c r="CO88" s="2"/>
-      <c r="DA88" s="26"/>
-      <c r="DB88" s="26" t="s">
+      <c r="DA88" s="8"/>
+      <c r="DB88" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="DC88" s="26"/>
-      <c r="DD88" s="26"/>
+      <c r="DC88" s="8"/>
+      <c r="DD88" s="8"/>
       <c r="DP88" s="2"/>
       <c r="FI88" s="2"/>
       <c r="FQ88" s="2"/>
@@ -2226,12 +2302,12 @@
       <c r="AO89" s="2"/>
       <c r="AW89" s="2"/>
       <c r="CO89" s="2"/>
-      <c r="DA89" s="26"/>
-      <c r="DB89" s="26" t="s">
+      <c r="DA89" s="8"/>
+      <c r="DB89" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="DC89" s="26"/>
-      <c r="DD89" s="26"/>
+      <c r="DC89" s="8"/>
+      <c r="DD89" s="8"/>
       <c r="DP89" s="2"/>
       <c r="FH89" s="2"/>
       <c r="FP89" s="2"/>
@@ -2254,12 +2330,12 @@
       <c r="AO90" s="2"/>
       <c r="AW90" s="2"/>
       <c r="CO90" s="2"/>
-      <c r="DA90" s="26"/>
-      <c r="DB90" s="26" t="s">
+      <c r="DA90" s="8"/>
+      <c r="DB90" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="DC90" s="26"/>
-      <c r="DD90" s="26"/>
+      <c r="DC90" s="8"/>
+      <c r="DD90" s="8"/>
       <c r="DP90" s="2"/>
       <c r="FH90" s="2"/>
       <c r="FP90" s="2"/>
@@ -2282,10 +2358,10 @@
       <c r="AO91" s="2"/>
       <c r="AW91" s="2"/>
       <c r="CO91" s="2"/>
-      <c r="DA91" s="26"/>
-      <c r="DB91" s="26"/>
-      <c r="DC91" s="26"/>
-      <c r="DD91" s="26"/>
+      <c r="DA91" s="8"/>
+      <c r="DB91" s="8"/>
+      <c r="DC91" s="8"/>
+      <c r="DD91" s="8"/>
       <c r="DP91" s="2"/>
       <c r="FH91" s="2"/>
       <c r="FP91" s="2"/>
@@ -4475,14 +4551,14 @@
       <c r="EI129" s="6"/>
       <c r="EJ129" s="6"/>
       <c r="EK129" s="6"/>
-      <c r="EL129" s="39"/>
-      <c r="EM129" s="39"/>
-      <c r="EN129" s="39"/>
-      <c r="EO129" s="39"/>
-      <c r="EP129" s="39"/>
-      <c r="EQ129" s="39"/>
-      <c r="ER129" s="39"/>
-      <c r="ES129" s="39"/>
+      <c r="EL129" s="9"/>
+      <c r="EM129" s="9"/>
+      <c r="EN129" s="9"/>
+      <c r="EO129" s="9"/>
+      <c r="EP129" s="9"/>
+      <c r="EQ129" s="9"/>
+      <c r="ER129" s="9"/>
+      <c r="ES129" s="9"/>
       <c r="ET129" s="6"/>
       <c r="EU129" s="6"/>
       <c r="EV129" s="6"/>
@@ -4630,14 +4706,14 @@
       <c r="EI130" s="6"/>
       <c r="EJ130" s="6"/>
       <c r="EK130" s="6"/>
-      <c r="EL130" s="39"/>
-      <c r="EM130" s="39"/>
-      <c r="EN130" s="39"/>
-      <c r="EO130" s="39"/>
-      <c r="EP130" s="39"/>
-      <c r="EQ130" s="39"/>
-      <c r="ER130" s="39"/>
-      <c r="ES130" s="39"/>
+      <c r="EL130" s="9"/>
+      <c r="EM130" s="9"/>
+      <c r="EN130" s="9"/>
+      <c r="EO130" s="9"/>
+      <c r="EP130" s="9"/>
+      <c r="EQ130" s="9"/>
+      <c r="ER130" s="9"/>
+      <c r="ES130" s="9"/>
       <c r="ET130" s="6"/>
       <c r="EU130" s="6"/>
       <c r="EV130" s="6"/>
@@ -4782,16 +4858,16 @@
       <c r="EI131" s="6"/>
       <c r="EJ131" s="6"/>
       <c r="EK131" s="6"/>
-      <c r="EL131" s="39"/>
-      <c r="EM131" s="39"/>
-      <c r="EN131" s="40" t="s">
+      <c r="EL131" s="9"/>
+      <c r="EM131" s="9"/>
+      <c r="EN131" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="EO131" s="41"/>
-      <c r="EP131" s="41"/>
-      <c r="EQ131" s="42"/>
-      <c r="ER131" s="39"/>
-      <c r="ES131" s="39"/>
+      <c r="EO131" s="11"/>
+      <c r="EP131" s="11"/>
+      <c r="EQ131" s="12"/>
+      <c r="ER131" s="9"/>
+      <c r="ES131" s="9"/>
       <c r="ET131" s="6"/>
       <c r="EU131" s="6"/>
       <c r="EV131" s="6"/>
@@ -4943,16 +5019,16 @@
       <c r="EI132" s="6"/>
       <c r="EJ132" s="6"/>
       <c r="EK132" s="6"/>
-      <c r="EL132" s="39"/>
-      <c r="EM132" s="39"/>
-      <c r="EN132" s="40" t="s">
+      <c r="EL132" s="9"/>
+      <c r="EM132" s="9"/>
+      <c r="EN132" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="EO132" s="41"/>
-      <c r="EP132" s="41"/>
-      <c r="EQ132" s="42"/>
-      <c r="ER132" s="39"/>
-      <c r="ES132" s="39"/>
+      <c r="EO132" s="11"/>
+      <c r="EP132" s="11"/>
+      <c r="EQ132" s="12"/>
+      <c r="ER132" s="9"/>
+      <c r="ES132" s="9"/>
       <c r="ET132" s="6"/>
       <c r="EU132" s="6"/>
       <c r="EV132" s="6"/>
@@ -5104,14 +5180,14 @@
       <c r="EI133" s="6"/>
       <c r="EJ133" s="6"/>
       <c r="EK133" s="6"/>
-      <c r="EL133" s="39"/>
-      <c r="EM133" s="39"/>
-      <c r="EN133" s="39"/>
-      <c r="EO133" s="39"/>
-      <c r="EP133" s="39"/>
-      <c r="EQ133" s="39"/>
-      <c r="ER133" s="39"/>
-      <c r="ES133" s="39"/>
+      <c r="EL133" s="9"/>
+      <c r="EM133" s="9"/>
+      <c r="EN133" s="9"/>
+      <c r="EO133" s="9"/>
+      <c r="EP133" s="9"/>
+      <c r="EQ133" s="9"/>
+      <c r="ER133" s="9"/>
+      <c r="ES133" s="9"/>
       <c r="ET133" s="6"/>
       <c r="EU133" s="6"/>
       <c r="EV133" s="6"/>
@@ -5263,14 +5339,14 @@
       <c r="EI134" s="6"/>
       <c r="EJ134" s="6"/>
       <c r="EK134" s="6"/>
-      <c r="EL134" s="39"/>
-      <c r="EM134" s="39"/>
-      <c r="EN134" s="39"/>
-      <c r="EO134" s="39"/>
-      <c r="EP134" s="39"/>
-      <c r="EQ134" s="39"/>
-      <c r="ER134" s="39"/>
-      <c r="ES134" s="39"/>
+      <c r="EL134" s="9"/>
+      <c r="EM134" s="9"/>
+      <c r="EN134" s="9"/>
+      <c r="EO134" s="9"/>
+      <c r="EP134" s="9"/>
+      <c r="EQ134" s="9"/>
+      <c r="ER134" s="9"/>
+      <c r="ES134" s="9"/>
       <c r="ET134" s="6"/>
       <c r="EU134" s="6"/>
       <c r="EV134" s="6"/>
@@ -5422,14 +5498,14 @@
       <c r="EI135" s="6"/>
       <c r="EJ135" s="6"/>
       <c r="EK135" s="6"/>
-      <c r="EL135" s="39"/>
-      <c r="EM135" s="39"/>
-      <c r="EN135" s="39"/>
-      <c r="EO135" s="39"/>
-      <c r="EP135" s="39"/>
-      <c r="EQ135" s="39"/>
-      <c r="ER135" s="39"/>
-      <c r="ES135" s="39"/>
+      <c r="EL135" s="9"/>
+      <c r="EM135" s="9"/>
+      <c r="EN135" s="9"/>
+      <c r="EO135" s="9"/>
+      <c r="EP135" s="9"/>
+      <c r="EQ135" s="9"/>
+      <c r="ER135" s="9"/>
+      <c r="ES135" s="9"/>
       <c r="ET135" s="6"/>
       <c r="EU135" s="6"/>
       <c r="EV135" s="6"/>
@@ -5581,14 +5657,14 @@
       <c r="EI136" s="6"/>
       <c r="EJ136" s="6"/>
       <c r="EK136" s="6"/>
-      <c r="EL136" s="39"/>
-      <c r="EM136" s="39"/>
-      <c r="EN136" s="39"/>
-      <c r="EO136" s="39"/>
-      <c r="EP136" s="39"/>
-      <c r="EQ136" s="39"/>
-      <c r="ER136" s="39"/>
-      <c r="ES136" s="39"/>
+      <c r="EL136" s="9"/>
+      <c r="EM136" s="9"/>
+      <c r="EN136" s="9"/>
+      <c r="EO136" s="9"/>
+      <c r="EP136" s="9"/>
+      <c r="EQ136" s="9"/>
+      <c r="ER136" s="9"/>
+      <c r="ES136" s="9"/>
       <c r="ET136" s="6"/>
       <c r="EU136" s="6"/>
       <c r="EV136" s="6"/>
@@ -5740,14 +5816,14 @@
       <c r="EI137" s="6"/>
       <c r="EJ137" s="6"/>
       <c r="EK137" s="6"/>
-      <c r="EL137" s="39"/>
-      <c r="EM137" s="39"/>
-      <c r="EN137" s="39"/>
-      <c r="EO137" s="39"/>
-      <c r="EP137" s="39"/>
-      <c r="EQ137" s="39"/>
-      <c r="ER137" s="39"/>
-      <c r="ES137" s="39"/>
+      <c r="EL137" s="9"/>
+      <c r="EM137" s="9"/>
+      <c r="EN137" s="9"/>
+      <c r="EO137" s="9"/>
+      <c r="EP137" s="9"/>
+      <c r="EQ137" s="9"/>
+      <c r="ER137" s="9"/>
+      <c r="ES137" s="9"/>
       <c r="ET137" s="6"/>
       <c r="EU137" s="6"/>
       <c r="EV137" s="6"/>
@@ -8897,7 +8973,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <webPublishItems count="2">
-    <webPublishItem id="25449" divId="CastleFloorPlan_25449" sourceType="sheet" destinationFile="D:\code\TanethPVE\CastleFloorPlan2.htm"/>
+    <webPublishItem id="25449" divId="CastleFloorPlan_25449" sourceType="sheet" destinationFile="D:\code\TanethPVE\CastleFloorPlan.htm"/>
     <webPublishItem id="4131" divId="CastleFloorPlan_4131" sourceType="range" sourceRef="B2:HE173" destinationFile="D:\code\TanethPVE\Temp\CastleFloorPlan.htm"/>
   </webPublishItems>
 </worksheet>

</xml_diff>